<commit_message>
feat: add insertion sort
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628F3956-A35B-41A6-B85B-5B9ADE08C4AA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819E3ECE-38D7-4474-93BE-1DEBFC9680AA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>bubble</t>
   </si>
@@ -32,6 +32,18 @@
   </si>
   <si>
     <t>18.02</t>
+  </si>
+  <si>
+    <t>insertion</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>0.127</t>
+  </si>
+  <si>
+    <t>12.892</t>
   </si>
 </sst>
 </file>
@@ -353,7 +365,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,10 +423,18 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>

</xml_diff>

<commit_message>
feat: add external sort 1
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E0C4AC-290D-41F5-9918-E16E65984CB1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A2954A-905B-4CBA-B772-2FD6B2F552C2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Random</t>
   </si>
@@ -110,6 +110,54 @@
   </si>
   <si>
     <t>9.095</t>
+  </si>
+  <si>
+    <t>ExternalSort1</t>
+  </si>
+  <si>
+    <t>0.007</t>
+  </si>
+  <si>
+    <t>0.014</t>
+  </si>
+  <si>
+    <t>0.009</t>
+  </si>
+  <si>
+    <t>0.011</t>
+  </si>
+  <si>
+    <t>0.015</t>
+  </si>
+  <si>
+    <t>0.020</t>
+  </si>
+  <si>
+    <t>0.072</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>0.100</t>
+  </si>
+  <si>
+    <t>0.766</t>
+  </si>
+  <si>
+    <t>0.838</t>
+  </si>
+  <si>
+    <t>0.924</t>
+  </si>
+  <si>
+    <t>8.453</t>
+  </si>
+  <si>
+    <t>9.232</t>
+  </si>
+  <si>
+    <t>10.119</t>
   </si>
 </sst>
 </file>
@@ -175,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -208,15 +256,30 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,43 +561,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="10">
+      <c r="B1" s="17">
         <v>100</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="13" t="s">
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="14" t="s">
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -573,13 +636,13 @@
       <c r="M2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="O2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="P2" s="14" t="s">
         <v>2</v>
       </c>
     </row>
@@ -623,13 +686,13 @@
       <c r="M3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="O3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="16" t="s">
         <v>16</v>
       </c>
     </row>
@@ -673,14 +736,114 @@
       <c r="M4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="N4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="O4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="16" t="s">
+      <c r="P4" s="15" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H5" s="22"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="10">
+        <v>5</v>
+      </c>
+      <c r="C6" s="10">
+        <v>10</v>
+      </c>
+      <c r="D6" s="10">
+        <v>15</v>
+      </c>
+      <c r="E6" s="11">
+        <v>5</v>
+      </c>
+      <c r="F6" s="11">
+        <v>10</v>
+      </c>
+      <c r="G6" s="11">
+        <v>15</v>
+      </c>
+      <c r="H6" s="12">
+        <v>5</v>
+      </c>
+      <c r="I6" s="12">
+        <v>10</v>
+      </c>
+      <c r="J6" s="12">
+        <v>15</v>
+      </c>
+      <c r="K6" s="13">
+        <v>5</v>
+      </c>
+      <c r="L6" s="13">
+        <v>10</v>
+      </c>
+      <c r="M6" s="13">
+        <v>15</v>
+      </c>
+      <c r="N6" s="16">
+        <v>5</v>
+      </c>
+      <c r="O6" s="16">
+        <v>10</v>
+      </c>
+      <c r="P6" s="16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="O7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="P7" s="15" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: change range of T
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A2954A-905B-4CBA-B772-2FD6B2F552C2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F992C5-E8C8-4FF8-B9EE-E32F281A7DF3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>Random</t>
   </si>
@@ -115,49 +115,49 @@
     <t>ExternalSort1</t>
   </si>
   <si>
-    <t>0.007</t>
-  </si>
-  <si>
-    <t>0.014</t>
-  </si>
-  <si>
-    <t>0.009</t>
-  </si>
-  <si>
-    <t>0.011</t>
-  </si>
-  <si>
-    <t>0.015</t>
-  </si>
-  <si>
-    <t>0.020</t>
-  </si>
-  <si>
-    <t>0.072</t>
-  </si>
-  <si>
-    <t>0.86</t>
-  </si>
-  <si>
-    <t>0.100</t>
-  </si>
-  <si>
-    <t>0.766</t>
-  </si>
-  <si>
-    <t>0.838</t>
-  </si>
-  <si>
-    <t>0.924</t>
-  </si>
-  <si>
-    <t>8.453</t>
-  </si>
-  <si>
-    <t>9.232</t>
-  </si>
-  <si>
-    <t>10.119</t>
+    <t>N</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>0.012</t>
+  </si>
+  <si>
+    <t>0.081</t>
+  </si>
+  <si>
+    <t>0.022</t>
+  </si>
+  <si>
+    <t>0.101</t>
+  </si>
+  <si>
+    <t>0.885</t>
+  </si>
+  <si>
+    <t>0.084</t>
+  </si>
+  <si>
+    <t>0.303</t>
+  </si>
+  <si>
+    <t>2.581</t>
+  </si>
+  <si>
+    <t>2.390</t>
+  </si>
+  <si>
+    <t>18.630</t>
+  </si>
+  <si>
+    <t>9.372</t>
+  </si>
+  <si>
+    <t>24.232</t>
+  </si>
+  <si>
+    <t>180.601</t>
   </si>
 </sst>
 </file>
@@ -173,7 +173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +207,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -223,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -244,18 +268,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -263,23 +275,54 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -561,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,31 +616,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="17">
+      <c r="B1" s="14">
         <v>100</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="20" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="21" t="s">
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -636,13 +679,13 @@
       <c r="M2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="10" t="s">
         <v>2</v>
       </c>
     </row>
@@ -686,13 +729,13 @@
       <c r="M3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="N3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="P3" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -736,118 +779,149 @@
       <c r="M4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="15" t="s">
+      <c r="N4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="15" t="s">
+      <c r="P4" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="H5" s="22"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B6" s="10">
-        <v>5</v>
-      </c>
-      <c r="C6" s="10">
-        <v>10</v>
-      </c>
-      <c r="D6" s="10">
-        <v>15</v>
-      </c>
-      <c r="E6" s="11">
-        <v>5</v>
-      </c>
-      <c r="F6" s="11">
-        <v>10</v>
-      </c>
-      <c r="G6" s="11">
-        <v>15</v>
-      </c>
-      <c r="H6" s="12">
-        <v>5</v>
-      </c>
-      <c r="I6" s="12">
-        <v>10</v>
-      </c>
-      <c r="J6" s="12">
-        <v>15</v>
-      </c>
-      <c r="K6" s="13">
-        <v>5</v>
-      </c>
-      <c r="L6" s="13">
-        <v>10</v>
-      </c>
-      <c r="M6" s="13">
-        <v>15</v>
-      </c>
-      <c r="N6" s="16">
-        <v>5</v>
-      </c>
-      <c r="O6" s="16">
-        <v>10</v>
-      </c>
-      <c r="P6" s="16">
-        <v>15</v>
-      </c>
+      <c r="H5" s="13"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="14">
+        <v>100</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="20">
+        <v>1000</v>
+      </c>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="23">
+        <v>10000</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1">
+        <v>100</v>
+      </c>
+      <c r="D8" s="21">
+        <v>10</v>
+      </c>
+      <c r="E8" s="21">
+        <v>100</v>
+      </c>
+      <c r="F8" s="21">
+        <v>1000</v>
+      </c>
+      <c r="G8" s="24">
+        <v>10</v>
+      </c>
+      <c r="H8" s="24">
+        <v>100</v>
+      </c>
+      <c r="I8" s="24">
+        <v>1000</v>
+      </c>
+      <c r="J8" s="27">
+        <v>10</v>
+      </c>
+      <c r="K8" s="27">
+        <v>100</v>
+      </c>
+      <c r="L8" s="27">
+        <v>1000</v>
+      </c>
+      <c r="M8" s="30">
+        <v>10</v>
+      </c>
+      <c r="N8" s="30">
+        <v>100</v>
+      </c>
+      <c r="O8" s="30">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="D9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="E9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="F9" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="G9" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="H9" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="I9" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="J9" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="L9" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="N7" s="15" t="s">
+      <c r="M9" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="O7" s="15" t="s">
+      <c r="N9" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="P7" s="15" t="s">
+      <c r="O9" s="31" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>

</xml_diff>